<commit_message>
Update newly subscripted variables in CID file
</commit_message>
<xml_diff>
--- a/InputData/web-app/CID/Check Input Data.xlsx
+++ b/InputData/web-app/CID/Check Input Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/todd/eps/eps-us/InputData/web-app/CID/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\web-app\CID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84AE5E4-3AE1-F642-BB0B-E244B9B3C3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163C0356-9559-4EF1-91ED-80F67B681CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60160" yWindow="500" windowWidth="30080" windowHeight="16660" activeTab="1" xr2:uid="{20505A23-B03E-B349-AF36-73B0855D7AFA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{20505A23-B03E-B349-AF36-73B0855D7AFA}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>CID Check Input Data</t>
   </si>
@@ -119,9 +119,6 @@
     <t>indst/IFStFS/IFStFS.csv</t>
   </si>
   <si>
-    <t>trans/BVTQaZ/BVTQaZ.csv</t>
-  </si>
-  <si>
     <t>trans/BVTStL/BVTStL.csv</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>trans/SRPbVT/SRPbVT.csv</t>
   </si>
   <si>
-    <t>trans/VTQaZ/VTQaZ.csv</t>
-  </si>
-  <si>
     <t>trans/VTStFES/VTStFES.csv</t>
   </si>
   <si>
@@ -156,6 +150,42 @@
   </si>
   <si>
     <t>trans/AVL/AVL.csv</t>
+  </si>
+  <si>
+    <t>trans/BVTQaZ/BVTQaZ-LDVs.csv</t>
+  </si>
+  <si>
+    <t>trans/BVTQaZ/BVTQaZ-HDVs.csv</t>
+  </si>
+  <si>
+    <t>trans/BVTQaZ/BVTQaZ-aircraft.csv</t>
+  </si>
+  <si>
+    <t>trans/BVTQaZ/BVTQaZ-rail.csv</t>
+  </si>
+  <si>
+    <t>trans/BVTQaZ/BVTQaZ-ships.csv</t>
+  </si>
+  <si>
+    <t>trans/BVTQaZ/BVTQaZ-motorbikes.csv</t>
+  </si>
+  <si>
+    <t>trans/VTQaZ/VTQaZ-LDVs.csv</t>
+  </si>
+  <si>
+    <t>trans/VTQaZ/VTQaZ-HDVs.csv</t>
+  </si>
+  <si>
+    <t>trans/VTQaZ/VTQaZ-aircraft.csv</t>
+  </si>
+  <si>
+    <t>trans/VTQaZ/VTQaZ-rail.csv</t>
+  </si>
+  <si>
+    <t>trans/VTQaZ/VTQaZ-ships.csv</t>
+  </si>
+  <si>
+    <t>trans/VTQaZ/VTQaZ-motorbikes.csv</t>
   </si>
 </sst>
 </file>
@@ -543,20 +573,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB40378-4D92-6B46-95EC-BF41FEF6A51A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="15.09765625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.69921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -564,14 +594,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -583,57 +613,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD815B91-4D8D-3140-B01A-98F4799EC5EA}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="20.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -643,126 +675,184 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C2FCA3-2250-8E45-A26E-181733CE1D14}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="32.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="24" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="25" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="26" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -774,35 +864,35 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="30.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>